<commit_message>
New example Graphics 2
</commit_message>
<xml_diff>
--- a/RStudio/First examples/BaseDatosCovid.xlsx
+++ b/RStudio/First examples/BaseDatosCovid.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="270">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="326">
   <si>
     <t>Fecha</t>
   </si>
@@ -425,6 +425,90 @@
     <t>133</t>
   </si>
   <si>
+    <t>134</t>
+  </si>
+  <si>
+    <t>135</t>
+  </si>
+  <si>
+    <t>136</t>
+  </si>
+  <si>
+    <t>137</t>
+  </si>
+  <si>
+    <t>138</t>
+  </si>
+  <si>
+    <t>139</t>
+  </si>
+  <si>
+    <t>140</t>
+  </si>
+  <si>
+    <t>141</t>
+  </si>
+  <si>
+    <t>142</t>
+  </si>
+  <si>
+    <t>143</t>
+  </si>
+  <si>
+    <t>144</t>
+  </si>
+  <si>
+    <t>145</t>
+  </si>
+  <si>
+    <t>146</t>
+  </si>
+  <si>
+    <t>147</t>
+  </si>
+  <si>
+    <t>148</t>
+  </si>
+  <si>
+    <t>149</t>
+  </si>
+  <si>
+    <t>150</t>
+  </si>
+  <si>
+    <t>151</t>
+  </si>
+  <si>
+    <t>152</t>
+  </si>
+  <si>
+    <t>153</t>
+  </si>
+  <si>
+    <t>154</t>
+  </si>
+  <si>
+    <t>155</t>
+  </si>
+  <si>
+    <t>156</t>
+  </si>
+  <si>
+    <t>157</t>
+  </si>
+  <si>
+    <t>158</t>
+  </si>
+  <si>
+    <t>159</t>
+  </si>
+  <si>
+    <t>160</t>
+  </si>
+  <si>
+    <t>161</t>
+  </si>
+  <si>
     <t>2020/03/05</t>
   </si>
   <si>
@@ -822,6 +906,90 @@
   </si>
   <si>
     <t>2020/07/15</t>
+  </si>
+  <si>
+    <t>2020/07/16</t>
+  </si>
+  <si>
+    <t>2020/07/17</t>
+  </si>
+  <si>
+    <t>2020/07/18</t>
+  </si>
+  <si>
+    <t>2020/07/19</t>
+  </si>
+  <si>
+    <t>2020/07/20</t>
+  </si>
+  <si>
+    <t>2020/07/21</t>
+  </si>
+  <si>
+    <t>2020/07/22</t>
+  </si>
+  <si>
+    <t>2020/07/23</t>
+  </si>
+  <si>
+    <t>2020/07/24</t>
+  </si>
+  <si>
+    <t>2020/07/25</t>
+  </si>
+  <si>
+    <t>2020/07/26</t>
+  </si>
+  <si>
+    <t>2020/07/27</t>
+  </si>
+  <si>
+    <t>2020/07/28</t>
+  </si>
+  <si>
+    <t>2020/07/29</t>
+  </si>
+  <si>
+    <t>2020/07/30</t>
+  </si>
+  <si>
+    <t>2020/07/31</t>
+  </si>
+  <si>
+    <t>2020/08/01</t>
+  </si>
+  <si>
+    <t>2020/08/02</t>
+  </si>
+  <si>
+    <t>2020/08/03</t>
+  </si>
+  <si>
+    <t>2020/08/04</t>
+  </si>
+  <si>
+    <t>2020/08/05</t>
+  </si>
+  <si>
+    <t>2020/08/06</t>
+  </si>
+  <si>
+    <t>2020/08/07</t>
+  </si>
+  <si>
+    <t>2020/08/08</t>
+  </si>
+  <si>
+    <t>2020/08/09</t>
+  </si>
+  <si>
+    <t>2020/08/10</t>
+  </si>
+  <si>
+    <t>2020/08/11</t>
+  </si>
+  <si>
+    <t>2020/08/12</t>
   </si>
 </sst>
 </file>
@@ -892,7 +1060,7 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>137</v>
+        <v>165</v>
       </c>
       <c r="C2" t="n">
         <v>0.0</v>
@@ -909,7 +1077,7 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>138</v>
+        <v>166</v>
       </c>
       <c r="C3" t="n">
         <v>1.0</v>
@@ -926,7 +1094,7 @@
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>139</v>
+        <v>167</v>
       </c>
       <c r="C4" t="n">
         <v>1.0</v>
@@ -943,7 +1111,7 @@
         <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>140</v>
+        <v>168</v>
       </c>
       <c r="C5" t="n">
         <v>5.0</v>
@@ -960,7 +1128,7 @@
         <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>141</v>
+        <v>169</v>
       </c>
       <c r="C6" t="n">
         <v>9.0</v>
@@ -977,7 +1145,7 @@
         <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>142</v>
+        <v>170</v>
       </c>
       <c r="C7" t="n">
         <v>9.0</v>
@@ -994,7 +1162,7 @@
         <v>10</v>
       </c>
       <c r="B8" t="s">
-        <v>143</v>
+        <v>171</v>
       </c>
       <c r="C8" t="n">
         <v>13.0</v>
@@ -1011,7 +1179,7 @@
         <v>11</v>
       </c>
       <c r="B9" t="s">
-        <v>144</v>
+        <v>172</v>
       </c>
       <c r="C9" t="n">
         <v>22.0</v>
@@ -1028,7 +1196,7 @@
         <v>12</v>
       </c>
       <c r="B10" t="s">
-        <v>145</v>
+        <v>173</v>
       </c>
       <c r="C10" t="n">
         <v>23.0</v>
@@ -1045,7 +1213,7 @@
         <v>13</v>
       </c>
       <c r="B11" t="s">
-        <v>146</v>
+        <v>174</v>
       </c>
       <c r="C11" t="n">
         <v>26.0</v>
@@ -1062,7 +1230,7 @@
         <v>14</v>
       </c>
       <c r="B12" t="s">
-        <v>147</v>
+        <v>175</v>
       </c>
       <c r="C12" t="n">
         <v>27.0</v>
@@ -1079,7 +1247,7 @@
         <v>15</v>
       </c>
       <c r="B13" t="s">
-        <v>148</v>
+        <v>176</v>
       </c>
       <c r="C13" t="n">
         <v>35.0</v>
@@ -1096,7 +1264,7 @@
         <v>16</v>
       </c>
       <c r="B14" t="s">
-        <v>149</v>
+        <v>177</v>
       </c>
       <c r="C14" t="n">
         <v>41.0</v>
@@ -1113,7 +1281,7 @@
         <v>17</v>
       </c>
       <c r="B15" t="s">
-        <v>150</v>
+        <v>178</v>
       </c>
       <c r="C15" t="n">
         <v>50.0</v>
@@ -1130,7 +1298,7 @@
         <v>18</v>
       </c>
       <c r="B16" t="s">
-        <v>151</v>
+        <v>179</v>
       </c>
       <c r="C16" t="n">
         <v>69.0</v>
@@ -1147,7 +1315,7 @@
         <v>19</v>
       </c>
       <c r="B17" t="s">
-        <v>152</v>
+        <v>180</v>
       </c>
       <c r="C17" t="n">
         <v>89.0</v>
@@ -1164,7 +1332,7 @@
         <v>20</v>
       </c>
       <c r="B18" t="s">
-        <v>153</v>
+        <v>181</v>
       </c>
       <c r="C18" t="n">
         <v>117.0</v>
@@ -1181,7 +1349,7 @@
         <v>21</v>
       </c>
       <c r="B19" t="s">
-        <v>154</v>
+        <v>182</v>
       </c>
       <c r="C19" t="n">
         <v>134.0</v>
@@ -1198,7 +1366,7 @@
         <v>22</v>
       </c>
       <c r="B20" t="s">
-        <v>155</v>
+        <v>183</v>
       </c>
       <c r="C20" t="n">
         <v>158.0</v>
@@ -1215,7 +1383,7 @@
         <v>23</v>
       </c>
       <c r="B21" t="s">
-        <v>156</v>
+        <v>184</v>
       </c>
       <c r="C21" t="n">
         <v>177.0</v>
@@ -1232,7 +1400,7 @@
         <v>24</v>
       </c>
       <c r="B22" t="s">
-        <v>157</v>
+        <v>185</v>
       </c>
       <c r="C22" t="n">
         <v>201.0</v>
@@ -1249,7 +1417,7 @@
         <v>25</v>
       </c>
       <c r="B23" t="s">
-        <v>158</v>
+        <v>186</v>
       </c>
       <c r="C23" t="n">
         <v>231.0</v>
@@ -1266,7 +1434,7 @@
         <v>26</v>
       </c>
       <c r="B24" t="s">
-        <v>159</v>
+        <v>187</v>
       </c>
       <c r="C24" t="n">
         <v>263.0</v>
@@ -1283,7 +1451,7 @@
         <v>27</v>
       </c>
       <c r="B25" t="s">
-        <v>160</v>
+        <v>188</v>
       </c>
       <c r="C25" t="n">
         <v>295.0</v>
@@ -1300,7 +1468,7 @@
         <v>28</v>
       </c>
       <c r="B26" t="s">
-        <v>161</v>
+        <v>189</v>
       </c>
       <c r="C26" t="n">
         <v>314.0</v>
@@ -1317,7 +1485,7 @@
         <v>29</v>
       </c>
       <c r="B27" t="s">
-        <v>162</v>
+        <v>190</v>
       </c>
       <c r="C27" t="n">
         <v>330.0</v>
@@ -1334,7 +1502,7 @@
         <v>30</v>
       </c>
       <c r="B28" t="s">
-        <v>163</v>
+        <v>191</v>
       </c>
       <c r="C28" t="n">
         <v>347.0</v>
@@ -1351,7 +1519,7 @@
         <v>31</v>
       </c>
       <c r="B29" t="s">
-        <v>164</v>
+        <v>192</v>
       </c>
       <c r="C29" t="n">
         <v>375.0</v>
@@ -1368,7 +1536,7 @@
         <v>32</v>
       </c>
       <c r="B30" t="s">
-        <v>165</v>
+        <v>193</v>
       </c>
       <c r="C30" t="n">
         <v>396.0</v>
@@ -1385,7 +1553,7 @@
         <v>33</v>
       </c>
       <c r="B31" t="s">
-        <v>166</v>
+        <v>194</v>
       </c>
       <c r="C31" t="n">
         <v>416.0</v>
@@ -1402,7 +1570,7 @@
         <v>34</v>
       </c>
       <c r="B32" t="s">
-        <v>167</v>
+        <v>195</v>
       </c>
       <c r="C32" t="n">
         <v>435.0</v>
@@ -1419,7 +1587,7 @@
         <v>35</v>
       </c>
       <c r="B33" t="s">
-        <v>168</v>
+        <v>196</v>
       </c>
       <c r="C33" t="n">
         <v>454.0</v>
@@ -1436,7 +1604,7 @@
         <v>36</v>
       </c>
       <c r="B34" t="s">
-        <v>169</v>
+        <v>197</v>
       </c>
       <c r="C34" t="n">
         <v>467.0</v>
@@ -1453,7 +1621,7 @@
         <v>37</v>
       </c>
       <c r="B35" t="s">
-        <v>170</v>
+        <v>198</v>
       </c>
       <c r="C35" t="n">
         <v>483.0</v>
@@ -1470,7 +1638,7 @@
         <v>38</v>
       </c>
       <c r="B36" t="s">
-        <v>171</v>
+        <v>199</v>
       </c>
       <c r="C36" t="n">
         <v>502.0</v>
@@ -1487,7 +1655,7 @@
         <v>39</v>
       </c>
       <c r="B37" t="s">
-        <v>172</v>
+        <v>200</v>
       </c>
       <c r="C37" t="n">
         <v>539.0</v>
@@ -1504,7 +1672,7 @@
         <v>40</v>
       </c>
       <c r="B38" t="s">
-        <v>173</v>
+        <v>201</v>
       </c>
       <c r="C38" t="n">
         <v>558.0</v>
@@ -1521,7 +1689,7 @@
         <v>41</v>
       </c>
       <c r="B39" t="s">
-        <v>174</v>
+        <v>202</v>
       </c>
       <c r="C39" t="n">
         <v>577.0</v>
@@ -1538,7 +1706,7 @@
         <v>42</v>
       </c>
       <c r="B40" t="s">
-        <v>175</v>
+        <v>203</v>
       </c>
       <c r="C40" t="n">
         <v>595.0</v>
@@ -1555,7 +1723,7 @@
         <v>43</v>
       </c>
       <c r="B41" t="s">
-        <v>176</v>
+        <v>204</v>
       </c>
       <c r="C41" t="n">
         <v>612.0</v>
@@ -1572,7 +1740,7 @@
         <v>44</v>
       </c>
       <c r="B42" t="s">
-        <v>177</v>
+        <v>205</v>
       </c>
       <c r="C42" t="n">
         <v>618.0</v>
@@ -1589,7 +1757,7 @@
         <v>45</v>
       </c>
       <c r="B43" t="s">
-        <v>178</v>
+        <v>206</v>
       </c>
       <c r="C43" t="n">
         <v>626.0</v>
@@ -1606,7 +1774,7 @@
         <v>46</v>
       </c>
       <c r="B44" t="s">
-        <v>179</v>
+        <v>207</v>
       </c>
       <c r="C44" t="n">
         <v>642.0</v>
@@ -1623,7 +1791,7 @@
         <v>47</v>
       </c>
       <c r="B45" t="s">
-        <v>180</v>
+        <v>208</v>
       </c>
       <c r="C45" t="n">
         <v>649.0</v>
@@ -1640,7 +1808,7 @@
         <v>48</v>
       </c>
       <c r="B46" t="s">
-        <v>181</v>
+        <v>209</v>
       </c>
       <c r="C46" t="n">
         <v>655.0</v>
@@ -1657,7 +1825,7 @@
         <v>49</v>
       </c>
       <c r="B47" t="s">
-        <v>182</v>
+        <v>210</v>
       </c>
       <c r="C47" t="n">
         <v>660.0</v>
@@ -1674,7 +1842,7 @@
         <v>50</v>
       </c>
       <c r="B48" t="s">
-        <v>183</v>
+        <v>211</v>
       </c>
       <c r="C48" t="n">
         <v>662.0</v>
@@ -1691,7 +1859,7 @@
         <v>51</v>
       </c>
       <c r="B49" t="s">
-        <v>184</v>
+        <v>212</v>
       </c>
       <c r="C49" t="n">
         <v>669.0</v>
@@ -1708,7 +1876,7 @@
         <v>52</v>
       </c>
       <c r="B50" t="s">
-        <v>185</v>
+        <v>213</v>
       </c>
       <c r="C50" t="n">
         <v>681.0</v>
@@ -1725,7 +1893,7 @@
         <v>53</v>
       </c>
       <c r="B51" t="s">
-        <v>186</v>
+        <v>214</v>
       </c>
       <c r="C51" t="n">
         <v>686.0</v>
@@ -1742,7 +1910,7 @@
         <v>54</v>
       </c>
       <c r="B52" t="s">
-        <v>187</v>
+        <v>215</v>
       </c>
       <c r="C52" t="n">
         <v>687.0</v>
@@ -1759,7 +1927,7 @@
         <v>55</v>
       </c>
       <c r="B53" t="s">
-        <v>188</v>
+        <v>216</v>
       </c>
       <c r="C53" t="n">
         <v>693.0</v>
@@ -1776,7 +1944,7 @@
         <v>56</v>
       </c>
       <c r="B54" t="s">
-        <v>189</v>
+        <v>217</v>
       </c>
       <c r="C54" t="n">
         <v>695.0</v>
@@ -1793,7 +1961,7 @@
         <v>57</v>
       </c>
       <c r="B55" t="s">
-        <v>190</v>
+        <v>218</v>
       </c>
       <c r="C55" t="n">
         <v>697.0</v>
@@ -1810,7 +1978,7 @@
         <v>58</v>
       </c>
       <c r="B56" t="s">
-        <v>191</v>
+        <v>219</v>
       </c>
       <c r="C56" t="n">
         <v>705.0</v>
@@ -1827,7 +1995,7 @@
         <v>59</v>
       </c>
       <c r="B57" t="s">
-        <v>192</v>
+        <v>220</v>
       </c>
       <c r="C57" t="n">
         <v>713.0</v>
@@ -1844,7 +2012,7 @@
         <v>60</v>
       </c>
       <c r="B58" t="s">
-        <v>193</v>
+        <v>221</v>
       </c>
       <c r="C58" t="n">
         <v>719.0</v>
@@ -1861,7 +2029,7 @@
         <v>61</v>
       </c>
       <c r="B59" t="s">
-        <v>194</v>
+        <v>222</v>
       </c>
       <c r="C59" t="n">
         <v>725.0</v>
@@ -1878,7 +2046,7 @@
         <v>62</v>
       </c>
       <c r="B60" t="s">
-        <v>195</v>
+        <v>223</v>
       </c>
       <c r="C60" t="n">
         <v>733.0</v>
@@ -1895,7 +2063,7 @@
         <v>63</v>
       </c>
       <c r="B61" t="s">
-        <v>196</v>
+        <v>224</v>
       </c>
       <c r="C61" t="n">
         <v>739.0</v>
@@ -1912,7 +2080,7 @@
         <v>64</v>
       </c>
       <c r="B62" t="s">
-        <v>197</v>
+        <v>225</v>
       </c>
       <c r="C62" t="n">
         <v>742.0</v>
@@ -1929,7 +2097,7 @@
         <v>65</v>
       </c>
       <c r="B63" t="s">
-        <v>198</v>
+        <v>226</v>
       </c>
       <c r="C63" t="n">
         <v>755.0</v>
@@ -1946,7 +2114,7 @@
         <v>66</v>
       </c>
       <c r="B64" t="s">
-        <v>199</v>
+        <v>227</v>
       </c>
       <c r="C64" t="n">
         <v>761.0</v>
@@ -1963,7 +2131,7 @@
         <v>67</v>
       </c>
       <c r="B65" t="s">
-        <v>200</v>
+        <v>228</v>
       </c>
       <c r="C65" t="n">
         <v>765.0</v>
@@ -1980,7 +2148,7 @@
         <v>68</v>
       </c>
       <c r="B66" t="s">
-        <v>201</v>
+        <v>229</v>
       </c>
       <c r="C66" t="n">
         <v>773.0</v>
@@ -1997,7 +2165,7 @@
         <v>69</v>
       </c>
       <c r="B67" t="s">
-        <v>202</v>
+        <v>230</v>
       </c>
       <c r="C67" t="n">
         <v>780.0</v>
@@ -2014,7 +2182,7 @@
         <v>70</v>
       </c>
       <c r="B68" t="s">
-        <v>203</v>
+        <v>231</v>
       </c>
       <c r="C68" t="n">
         <v>792.0</v>
@@ -2031,7 +2199,7 @@
         <v>71</v>
       </c>
       <c r="B69" t="s">
-        <v>204</v>
+        <v>232</v>
       </c>
       <c r="C69" t="n">
         <v>801.0</v>
@@ -2048,7 +2216,7 @@
         <v>72</v>
       </c>
       <c r="B70" t="s">
-        <v>205</v>
+        <v>233</v>
       </c>
       <c r="C70" t="n">
         <v>804.0</v>
@@ -2065,7 +2233,7 @@
         <v>73</v>
       </c>
       <c r="B71" t="s">
-        <v>206</v>
+        <v>234</v>
       </c>
       <c r="C71" t="n">
         <v>815.0</v>
@@ -2082,7 +2250,7 @@
         <v>74</v>
       </c>
       <c r="B72" t="s">
-        <v>207</v>
+        <v>235</v>
       </c>
       <c r="C72" t="n">
         <v>830.0</v>
@@ -2099,7 +2267,7 @@
         <v>75</v>
       </c>
       <c r="B73" t="s">
-        <v>208</v>
+        <v>236</v>
       </c>
       <c r="C73" t="n">
         <v>843.0</v>
@@ -2116,7 +2284,7 @@
         <v>76</v>
       </c>
       <c r="B74" t="s">
-        <v>209</v>
+        <v>237</v>
       </c>
       <c r="C74" t="n">
         <v>853.0</v>
@@ -2133,7 +2301,7 @@
         <v>77</v>
       </c>
       <c r="B75" t="s">
-        <v>210</v>
+        <v>238</v>
       </c>
       <c r="C75" t="n">
         <v>863.0</v>
@@ -2150,7 +2318,7 @@
         <v>78</v>
       </c>
       <c r="B76" t="s">
-        <v>211</v>
+        <v>239</v>
       </c>
       <c r="C76" t="n">
         <v>866.0</v>
@@ -2167,7 +2335,7 @@
         <v>79</v>
       </c>
       <c r="B77" t="s">
-        <v>212</v>
+        <v>240</v>
       </c>
       <c r="C77" t="n">
         <v>882.0</v>
@@ -2184,7 +2352,7 @@
         <v>80</v>
       </c>
       <c r="B78" t="s">
-        <v>213</v>
+        <v>241</v>
       </c>
       <c r="C78" t="n">
         <v>897.0</v>
@@ -2201,7 +2369,7 @@
         <v>81</v>
       </c>
       <c r="B79" t="s">
-        <v>214</v>
+        <v>242</v>
       </c>
       <c r="C79" t="n">
         <v>903.0</v>
@@ -2218,7 +2386,7 @@
         <v>82</v>
       </c>
       <c r="B80" t="s">
-        <v>215</v>
+        <v>243</v>
       </c>
       <c r="C80" t="n">
         <v>911.0</v>
@@ -2235,7 +2403,7 @@
         <v>83</v>
       </c>
       <c r="B81" t="s">
-        <v>216</v>
+        <v>244</v>
       </c>
       <c r="C81" t="n">
         <v>918.0</v>
@@ -2252,7 +2420,7 @@
         <v>84</v>
       </c>
       <c r="B82" t="s">
-        <v>217</v>
+        <v>245</v>
       </c>
       <c r="C82" t="n">
         <v>930.0</v>
@@ -2269,7 +2437,7 @@
         <v>85</v>
       </c>
       <c r="B83" t="s">
-        <v>218</v>
+        <v>246</v>
       </c>
       <c r="C83" t="n">
         <v>951.0</v>
@@ -2286,7 +2454,7 @@
         <v>86</v>
       </c>
       <c r="B84" t="s">
-        <v>219</v>
+        <v>247</v>
       </c>
       <c r="C84" t="n">
         <v>956.0</v>
@@ -2303,7 +2471,7 @@
         <v>87</v>
       </c>
       <c r="B85" t="s">
-        <v>220</v>
+        <v>248</v>
       </c>
       <c r="C85" t="n">
         <v>984.0</v>
@@ -2320,7 +2488,7 @@
         <v>88</v>
       </c>
       <c r="B86" t="s">
-        <v>221</v>
+        <v>249</v>
       </c>
       <c r="C86" t="n">
         <v>1000.0</v>
@@ -2337,7 +2505,7 @@
         <v>89</v>
       </c>
       <c r="B87" t="s">
-        <v>222</v>
+        <v>250</v>
       </c>
       <c r="C87" t="n">
         <v>1022.0</v>
@@ -2354,7 +2522,7 @@
         <v>90</v>
       </c>
       <c r="B88" t="s">
-        <v>223</v>
+        <v>251</v>
       </c>
       <c r="C88" t="n">
         <v>1047.0</v>
@@ -2371,7 +2539,7 @@
         <v>91</v>
       </c>
       <c r="B89" t="s">
-        <v>224</v>
+        <v>252</v>
       </c>
       <c r="C89" t="n">
         <v>1056.0</v>
@@ -2388,7 +2556,7 @@
         <v>92</v>
       </c>
       <c r="B90" t="s">
-        <v>225</v>
+        <v>253</v>
       </c>
       <c r="C90" t="n">
         <v>1084.0</v>
@@ -2405,7 +2573,7 @@
         <v>93</v>
       </c>
       <c r="B91" t="s">
-        <v>226</v>
+        <v>254</v>
       </c>
       <c r="C91" t="n">
         <v>1105.0</v>
@@ -2422,7 +2590,7 @@
         <v>94</v>
       </c>
       <c r="B92" t="s">
-        <v>227</v>
+        <v>255</v>
       </c>
       <c r="C92" t="n">
         <v>1157.0</v>
@@ -2439,7 +2607,7 @@
         <v>95</v>
       </c>
       <c r="B93" t="s">
-        <v>228</v>
+        <v>256</v>
       </c>
       <c r="C93" t="n">
         <v>1194.0</v>
@@ -2456,7 +2624,7 @@
         <v>96</v>
       </c>
       <c r="B94" t="s">
-        <v>229</v>
+        <v>257</v>
       </c>
       <c r="C94" t="n">
         <v>1228.0</v>
@@ -2473,7 +2641,7 @@
         <v>97</v>
       </c>
       <c r="B95" t="s">
-        <v>230</v>
+        <v>258</v>
       </c>
       <c r="C95" t="n">
         <v>1263.0</v>
@@ -2490,7 +2658,7 @@
         <v>98</v>
       </c>
       <c r="B96" t="s">
-        <v>231</v>
+        <v>259</v>
       </c>
       <c r="C96" t="n">
         <v>1318.0</v>
@@ -2507,7 +2675,7 @@
         <v>99</v>
       </c>
       <c r="B97" t="s">
-        <v>232</v>
+        <v>260</v>
       </c>
       <c r="C97" t="n">
         <v>1342.0</v>
@@ -2524,7 +2692,7 @@
         <v>100</v>
       </c>
       <c r="B98" t="s">
-        <v>233</v>
+        <v>261</v>
       </c>
       <c r="C98" t="n">
         <v>1375.0</v>
@@ -2541,7 +2709,7 @@
         <v>101</v>
       </c>
       <c r="B99" t="s">
-        <v>234</v>
+        <v>262</v>
       </c>
       <c r="C99" t="n">
         <v>1461.0</v>
@@ -2558,7 +2726,7 @@
         <v>102</v>
       </c>
       <c r="B100" t="s">
-        <v>235</v>
+        <v>263</v>
       </c>
       <c r="C100" t="n">
         <v>1538.0</v>
@@ -2575,7 +2743,7 @@
         <v>103</v>
       </c>
       <c r="B101" t="s">
-        <v>236</v>
+        <v>264</v>
       </c>
       <c r="C101" t="n">
         <v>1612.0</v>
@@ -2592,7 +2760,7 @@
         <v>104</v>
       </c>
       <c r="B102" t="s">
-        <v>237</v>
+        <v>265</v>
       </c>
       <c r="C102" t="n">
         <v>1662.0</v>
@@ -2609,7 +2777,7 @@
         <v>105</v>
       </c>
       <c r="B103" t="s">
-        <v>238</v>
+        <v>266</v>
       </c>
       <c r="C103" t="n">
         <v>1715.0</v>
@@ -2626,7 +2794,7 @@
         <v>106</v>
       </c>
       <c r="B104" t="s">
-        <v>239</v>
+        <v>267</v>
       </c>
       <c r="C104" t="n">
         <v>1744.0</v>
@@ -2643,7 +2811,7 @@
         <v>107</v>
       </c>
       <c r="B105" t="s">
-        <v>240</v>
+        <v>268</v>
       </c>
       <c r="C105" t="n">
         <v>1796.0</v>
@@ -2660,7 +2828,7 @@
         <v>108</v>
       </c>
       <c r="B106" t="s">
-        <v>241</v>
+        <v>269</v>
       </c>
       <c r="C106" t="n">
         <v>1871.0</v>
@@ -2677,7 +2845,7 @@
         <v>109</v>
       </c>
       <c r="B107" t="s">
-        <v>242</v>
+        <v>270</v>
       </c>
       <c r="C107" t="n">
         <v>1939.0</v>
@@ -2694,7 +2862,7 @@
         <v>110</v>
       </c>
       <c r="B108" t="s">
-        <v>243</v>
+        <v>271</v>
       </c>
       <c r="C108" t="n">
         <v>2058.0</v>
@@ -2711,7 +2879,7 @@
         <v>111</v>
       </c>
       <c r="B109" t="s">
-        <v>244</v>
+        <v>272</v>
       </c>
       <c r="C109" t="n">
         <v>2127.0</v>
@@ -2728,7 +2896,7 @@
         <v>112</v>
       </c>
       <c r="B110" t="s">
-        <v>245</v>
+        <v>273</v>
       </c>
       <c r="C110" t="n">
         <v>2213.0</v>
@@ -2745,7 +2913,7 @@
         <v>113</v>
       </c>
       <c r="B111" t="s">
-        <v>246</v>
+        <v>274</v>
       </c>
       <c r="C111" t="n">
         <v>2277.0</v>
@@ -2762,7 +2930,7 @@
         <v>114</v>
       </c>
       <c r="B112" t="s">
-        <v>247</v>
+        <v>275</v>
       </c>
       <c r="C112" t="n">
         <v>2368.0</v>
@@ -2779,7 +2947,7 @@
         <v>115</v>
       </c>
       <c r="B113" t="s">
-        <v>248</v>
+        <v>276</v>
       </c>
       <c r="C113" t="n">
         <v>2515.0</v>
@@ -2796,7 +2964,7 @@
         <v>116</v>
       </c>
       <c r="B114" t="s">
-        <v>249</v>
+        <v>277</v>
       </c>
       <c r="C114" t="n">
         <v>2684.0</v>
@@ -2813,7 +2981,7 @@
         <v>117</v>
       </c>
       <c r="B115" t="s">
-        <v>250</v>
+        <v>278</v>
       </c>
       <c r="C115" t="n">
         <v>2836.0</v>
@@ -2830,7 +2998,7 @@
         <v>118</v>
       </c>
       <c r="B116" t="s">
-        <v>251</v>
+        <v>279</v>
       </c>
       <c r="C116" t="n">
         <v>2979.0</v>
@@ -2847,7 +3015,7 @@
         <v>119</v>
       </c>
       <c r="B117" t="s">
-        <v>252</v>
+        <v>280</v>
       </c>
       <c r="C117" t="n">
         <v>3130.0</v>
@@ -2864,7 +3032,7 @@
         <v>120</v>
       </c>
       <c r="B118" t="s">
-        <v>253</v>
+        <v>281</v>
       </c>
       <c r="C118" t="n">
         <v>3269.0</v>
@@ -2881,7 +3049,7 @@
         <v>121</v>
       </c>
       <c r="B119" t="s">
-        <v>254</v>
+        <v>282</v>
       </c>
       <c r="C119" t="n">
         <v>3459.0</v>
@@ -2898,7 +3066,7 @@
         <v>122</v>
       </c>
       <c r="B120" t="s">
-        <v>255</v>
+        <v>283</v>
       </c>
       <c r="C120" t="n">
         <v>3753.0</v>
@@ -2915,7 +3083,7 @@
         <v>123</v>
       </c>
       <c r="B121" t="s">
-        <v>256</v>
+        <v>284</v>
       </c>
       <c r="C121" t="n">
         <v>4023.0</v>
@@ -2932,7 +3100,7 @@
         <v>124</v>
       </c>
       <c r="B122" t="s">
-        <v>257</v>
+        <v>285</v>
       </c>
       <c r="C122" t="n">
         <v>4311.0</v>
@@ -2949,7 +3117,7 @@
         <v>125</v>
       </c>
       <c r="B123" t="s">
-        <v>258</v>
+        <v>286</v>
       </c>
       <c r="C123" t="n">
         <v>4621.0</v>
@@ -2966,7 +3134,7 @@
         <v>126</v>
       </c>
       <c r="B124" t="s">
-        <v>259</v>
+        <v>287</v>
       </c>
       <c r="C124" t="n">
         <v>4996.0</v>
@@ -2983,7 +3151,7 @@
         <v>127</v>
       </c>
       <c r="B125" t="s">
-        <v>260</v>
+        <v>288</v>
       </c>
       <c r="C125" t="n">
         <v>5241.0</v>
@@ -3000,7 +3168,7 @@
         <v>128</v>
       </c>
       <c r="B126" t="s">
-        <v>261</v>
+        <v>289</v>
       </c>
       <c r="C126" t="n">
         <v>5486.0</v>
@@ -3017,7 +3185,7 @@
         <v>129</v>
       </c>
       <c r="B127" t="s">
-        <v>262</v>
+        <v>290</v>
       </c>
       <c r="C127" t="n">
         <v>5836.0</v>
@@ -3034,7 +3202,7 @@
         <v>130</v>
       </c>
       <c r="B128" t="s">
-        <v>263</v>
+        <v>291</v>
       </c>
       <c r="C128" t="n">
         <v>6485.0</v>
@@ -3051,7 +3219,7 @@
         <v>131</v>
       </c>
       <c r="B129" t="s">
-        <v>264</v>
+        <v>292</v>
       </c>
       <c r="C129" t="n">
         <v>6845.0</v>
@@ -3068,7 +3236,7 @@
         <v>132</v>
       </c>
       <c r="B130" t="s">
-        <v>265</v>
+        <v>293</v>
       </c>
       <c r="C130" t="n">
         <v>7231.0</v>
@@ -3085,7 +3253,7 @@
         <v>133</v>
       </c>
       <c r="B131" t="s">
-        <v>266</v>
+        <v>294</v>
       </c>
       <c r="C131" t="n">
         <v>7596.0</v>
@@ -3102,7 +3270,7 @@
         <v>134</v>
       </c>
       <c r="B132" t="s">
-        <v>267</v>
+        <v>295</v>
       </c>
       <c r="C132" t="n">
         <v>8036.0</v>
@@ -3119,7 +3287,7 @@
         <v>135</v>
       </c>
       <c r="B133" t="s">
-        <v>268</v>
+        <v>296</v>
       </c>
       <c r="C133" t="n">
         <v>8482.0</v>
@@ -3136,7 +3304,7 @@
         <v>136</v>
       </c>
       <c r="B134" t="s">
-        <v>269</v>
+        <v>297</v>
       </c>
       <c r="C134" t="n">
         <v>8986.0</v>
@@ -3146,6 +3314,482 @@
       </c>
       <c r="E134" t="n">
         <v>583.46</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="s">
+        <v>137</v>
+      </c>
+      <c r="B135" t="s">
+        <v>298</v>
+      </c>
+      <c r="C135" t="n">
+        <v>9546.0</v>
+      </c>
+      <c r="D135" t="n">
+        <v>578.74</v>
+      </c>
+      <c r="E135" t="n">
+        <v>582.86</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="s">
+        <v>138</v>
+      </c>
+      <c r="B136" t="s">
+        <v>299</v>
+      </c>
+      <c r="C136" t="n">
+        <v>9969.0</v>
+      </c>
+      <c r="D136" t="n">
+        <v>578.91</v>
+      </c>
+      <c r="E136" t="n">
+        <v>584.16</v>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="s">
+        <v>139</v>
+      </c>
+      <c r="B137" t="s">
+        <v>300</v>
+      </c>
+      <c r="C137" t="n">
+        <v>10551.0</v>
+      </c>
+      <c r="D137" t="n">
+        <v>578.7</v>
+      </c>
+      <c r="E137" t="n">
+        <v>584.52</v>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="s">
+        <v>140</v>
+      </c>
+      <c r="B138" t="s">
+        <v>301</v>
+      </c>
+      <c r="C138" t="n">
+        <v>11114.0</v>
+      </c>
+      <c r="D138" t="n">
+        <v>578.7</v>
+      </c>
+      <c r="E138" t="n">
+        <v>584.52</v>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="s">
+        <v>141</v>
+      </c>
+      <c r="B139" t="s">
+        <v>302</v>
+      </c>
+      <c r="C139" t="n">
+        <v>11534.0</v>
+      </c>
+      <c r="D139" t="n">
+        <v>578.7</v>
+      </c>
+      <c r="E139" t="n">
+        <v>584.52</v>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="s">
+        <v>142</v>
+      </c>
+      <c r="B140" t="s">
+        <v>303</v>
+      </c>
+      <c r="C140" t="n">
+        <v>11811.0</v>
+      </c>
+      <c r="D140" t="n">
+        <v>576.47</v>
+      </c>
+      <c r="E140" t="n">
+        <v>584.94</v>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="s">
+        <v>143</v>
+      </c>
+      <c r="B141" t="s">
+        <v>304</v>
+      </c>
+      <c r="C141" t="n">
+        <v>12361.0</v>
+      </c>
+      <c r="D141" t="n">
+        <v>576.73</v>
+      </c>
+      <c r="E141" t="n">
+        <v>585.21</v>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="s">
+        <v>144</v>
+      </c>
+      <c r="B142" t="s">
+        <v>305</v>
+      </c>
+      <c r="C142" t="n">
+        <v>13129.0</v>
+      </c>
+      <c r="D142" t="n">
+        <v>579.78</v>
+      </c>
+      <c r="E142" t="n">
+        <v>585.62</v>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="s">
+        <v>145</v>
+      </c>
+      <c r="B143" t="s">
+        <v>306</v>
+      </c>
+      <c r="C143" t="n">
+        <v>13669.0</v>
+      </c>
+      <c r="D143" t="n">
+        <v>579.6</v>
+      </c>
+      <c r="E143" t="n">
+        <v>586.01</v>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="s">
+        <v>146</v>
+      </c>
+      <c r="B144" t="s">
+        <v>307</v>
+      </c>
+      <c r="C144" t="n">
+        <v>14600.0</v>
+      </c>
+      <c r="D144" t="n">
+        <v>579.69</v>
+      </c>
+      <c r="E144" t="n">
+        <v>586.27</v>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="s">
+        <v>147</v>
+      </c>
+      <c r="B145" t="s">
+        <v>308</v>
+      </c>
+      <c r="C145" t="n">
+        <v>15229.0</v>
+      </c>
+      <c r="D145" t="n">
+        <v>579.69</v>
+      </c>
+      <c r="E145" t="n">
+        <v>586.27</v>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="s">
+        <v>148</v>
+      </c>
+      <c r="B146" t="s">
+        <v>309</v>
+      </c>
+      <c r="C146" t="n">
+        <v>15841.0</v>
+      </c>
+      <c r="D146" t="n">
+        <v>579.69</v>
+      </c>
+      <c r="E146" t="n">
+        <v>586.27</v>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" t="s">
+        <v>149</v>
+      </c>
+      <c r="B147" t="s">
+        <v>310</v>
+      </c>
+      <c r="C147" t="n">
+        <v>16344.0</v>
+      </c>
+      <c r="D147" t="n">
+        <v>579.69</v>
+      </c>
+      <c r="E147" t="n">
+        <v>586.27</v>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" t="s">
+        <v>150</v>
+      </c>
+      <c r="B148" t="s">
+        <v>311</v>
+      </c>
+      <c r="C148" t="n">
+        <v>16800.0</v>
+      </c>
+      <c r="D148" t="n">
+        <v>580.49</v>
+      </c>
+      <c r="E148" t="n">
+        <v>586.9</v>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="s">
+        <v>151</v>
+      </c>
+      <c r="B149" t="s">
+        <v>312</v>
+      </c>
+      <c r="C149" t="n">
+        <v>17290.0</v>
+      </c>
+      <c r="D149" t="n">
+        <v>580.51</v>
+      </c>
+      <c r="E149" t="n">
+        <v>586.91</v>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" t="s">
+        <v>152</v>
+      </c>
+      <c r="B150" t="s">
+        <v>313</v>
+      </c>
+      <c r="C150" t="n">
+        <v>17820.0</v>
+      </c>
+      <c r="D150" t="n">
+        <v>582.15</v>
+      </c>
+      <c r="E150" t="n">
+        <v>588.33</v>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" t="s">
+        <v>153</v>
+      </c>
+      <c r="B151" t="s">
+        <v>314</v>
+      </c>
+      <c r="C151" t="n">
+        <v>18187.0</v>
+      </c>
+      <c r="D151" t="n">
+        <v>582.41</v>
+      </c>
+      <c r="E151" t="n">
+        <v>590.74</v>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" t="s">
+        <v>154</v>
+      </c>
+      <c r="B152" t="s">
+        <v>315</v>
+      </c>
+      <c r="C152" t="n">
+        <v>18975.0</v>
+      </c>
+      <c r="D152" t="n">
+        <v>582.41</v>
+      </c>
+      <c r="E152" t="n">
+        <v>590.74</v>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" t="s">
+        <v>155</v>
+      </c>
+      <c r="B153" t="s">
+        <v>316</v>
+      </c>
+      <c r="C153" t="n">
+        <v>19402.0</v>
+      </c>
+      <c r="D153" t="n">
+        <v>582.41</v>
+      </c>
+      <c r="E153" t="n">
+        <v>590.74</v>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" t="s">
+        <v>156</v>
+      </c>
+      <c r="B154" t="s">
+        <v>317</v>
+      </c>
+      <c r="C154" t="n">
+        <v>19837.0</v>
+      </c>
+      <c r="D154" t="n">
+        <v>584.23</v>
+      </c>
+      <c r="E154" t="n">
+        <v>592.22</v>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" t="s">
+        <v>157</v>
+      </c>
+      <c r="B155" t="s">
+        <v>318</v>
+      </c>
+      <c r="C155" t="n">
+        <v>20417.0</v>
+      </c>
+      <c r="D155" t="n">
+        <v>586.65</v>
+      </c>
+      <c r="E155" t="n">
+        <v>594.44</v>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" t="s">
+        <v>158</v>
+      </c>
+      <c r="B156" t="s">
+        <v>319</v>
+      </c>
+      <c r="C156" t="n">
+        <v>21070.0</v>
+      </c>
+      <c r="D156" t="n">
+        <v>588.12</v>
+      </c>
+      <c r="E156" t="n">
+        <v>595.21</v>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" t="s">
+        <v>159</v>
+      </c>
+      <c r="B157" t="s">
+        <v>320</v>
+      </c>
+      <c r="C157" t="n">
+        <v>22081.0</v>
+      </c>
+      <c r="D157" t="n">
+        <v>588.7</v>
+      </c>
+      <c r="E157" t="n">
+        <v>596.17</v>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" t="s">
+        <v>160</v>
+      </c>
+      <c r="B158" t="s">
+        <v>321</v>
+      </c>
+      <c r="C158" t="n">
+        <v>22802.0</v>
+      </c>
+      <c r="D158" t="n">
+        <v>588.22</v>
+      </c>
+      <c r="E158" t="n">
+        <v>595.91</v>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" t="s">
+        <v>161</v>
+      </c>
+      <c r="B159" t="s">
+        <v>322</v>
+      </c>
+      <c r="C159" t="n">
+        <v>23286.0</v>
+      </c>
+      <c r="D159" t="n">
+        <v>588.22</v>
+      </c>
+      <c r="E159" t="n">
+        <v>595.91</v>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" t="s">
+        <v>162</v>
+      </c>
+      <c r="B160" t="s">
+        <v>323</v>
+      </c>
+      <c r="C160" t="n">
+        <v>23872.0</v>
+      </c>
+      <c r="D160" t="n">
+        <v>588.22</v>
+      </c>
+      <c r="E160" t="n">
+        <v>595.91</v>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" t="s">
+        <v>163</v>
+      </c>
+      <c r="B161" t="s">
+        <v>324</v>
+      </c>
+      <c r="C161" t="n">
+        <v>24508.0</v>
+      </c>
+      <c r="D161" t="n">
+        <v>590.69</v>
+      </c>
+      <c r="E161" t="n">
+        <v>598.21</v>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" t="s">
+        <v>164</v>
+      </c>
+      <c r="B162" t="s">
+        <v>325</v>
+      </c>
+      <c r="C162" t="n">
+        <v>25057.0</v>
+      </c>
+      <c r="D162" t="n">
+        <v>592.54</v>
+      </c>
+      <c r="E162" t="n">
+        <v>599.13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>